<commit_message>
ng: update TAS1 forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Nigeria/ng_lf_tas_3_resultat_fts_202202.xlsx
+++ b/LF/TAS/Nigeria/ng_lf_tas_3_resultat_fts_202202.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12240" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -313,37 +313,37 @@
     <t>why_invalid</t>
   </si>
   <si>
-    <t>Absence.de.ligne.temoin/controle</t>
+    <t>Absence.of.control.line</t>
   </si>
   <si>
     <t>Absence of control line</t>
   </si>
   <si>
-    <t>Ligne.temoin.discontinue/partielle</t>
+    <t>Broken/partial.control.line</t>
   </si>
   <si>
     <t>Broken/partial control line</t>
   </si>
   <si>
-    <t>Difficulte.d’absorption.d’echantillon</t>
+    <t>Difficulty.of.absorbing.sample</t>
   </si>
   <si>
     <t>Difficulty of absorbing sample</t>
   </si>
   <si>
-    <t>Difficulte.de.migration.d’echantillon</t>
+    <t>Difficulty.of.migrating.sample</t>
   </si>
   <si>
     <t>Difficulty of migrating sample</t>
   </si>
   <si>
-    <t>Trace.de.sang.persiste.(sang.reste.sur.la.bandelette/a.obscurci.les.lignes)</t>
+    <t>Trace.of.blood.persists</t>
   </si>
   <si>
     <t>Trace of blood persists</t>
   </si>
   <si>
-    <t>Insuffisance.du.volume.de.sang.du.a.la.pipette</t>
+    <t>Insufficient.blood.volume.due.to.pipette</t>
   </si>
   <si>
     <t>Insufficient blood volume due to pipette</t>
@@ -1414,7 +1414,7 @@
   <sheetPr/>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -1978,10 +1978,10 @@
   <sheetPr/>
   <dimension ref="A1:F323"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D$1:D$1048576"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="5"/>

</xml_diff>